<commit_message>
Char.py working, now adding characters
</commit_message>
<xml_diff>
--- a/Characters/Characters.xlsx
+++ b/Characters/Characters.xlsx
@@ -461,7 +461,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="0" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
@@ -529,31 +529,80 @@
       </c>
     </row>
     <row r="3" ht="13.8" customHeight="1" s="5">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="4" t="inlineStr">
         <is>
           <t>Lulo Tsuzaki</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="B3" s="4" t="n">
         <v>17</v>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" s="4" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="D3" s="4" t="inlineStr">
         <is>
           <t>Mythicals</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="E3" s="4" t="inlineStr">
         <is>
           <t>Secondary MC</t>
         </is>
       </c>
     </row>
-    <row r="4" ht="13.8" customHeight="1" s="5"/>
+    <row r="4" ht="13.8" customHeight="1" s="5">
+      <c r="A4" s="4" t="inlineStr">
+        <is>
+          <t>Khloe Bright</t>
+        </is>
+      </c>
+      <c r="B4" s="4" t="n">
+        <v>18</v>
+      </c>
+      <c r="C4" s="4" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D4" s="4" t="inlineStr">
+        <is>
+          <t>Insects</t>
+        </is>
+      </c>
+      <c r="E4" s="4" t="inlineStr">
+        <is>
+          <t>Female Bestfriend</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Percy Thomson</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>17</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Mythicals(Elves)</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Comical Partner</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>